<commit_message>
Correction to cargo distance conversion factor
</commit_message>
<xml_diff>
--- a/InputData/web-app/CDCF/Cargo Dist Conversion Factors.xlsx
+++ b/InputData/web-app/CDCF/Cargo Dist Conversion Factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deept\OneDrive\Desktop\India InputData 5-6-2020\web-app\CDCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-mexico\InputData\web-app\CDCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2315D679-75BF-456D-9B52-FDDF8539BBEB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F496BAC-E30A-42D5-96AA-0476CB43D7F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -59,9 +63,6 @@
     <t>CDCF Freight Ton Miles per Freight Distance Output Unit</t>
   </si>
   <si>
-    <t>For the India model, the desired output units are:</t>
-  </si>
-  <si>
     <t>trillion passenger-kilometers</t>
   </si>
   <si>
@@ -78,6 +79,9 @@
   </si>
   <si>
     <t>freight ton-kilometers</t>
+  </si>
+  <si>
+    <t>For the Mexico model, the desired output units are:</t>
   </si>
 </sst>
 </file>
@@ -480,70 +484,70 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -566,24 +570,23 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.26953125" customWidth="1"/>
+    <col min="2" max="2" width="28.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2">
-        <f>1.60934*10^12</f>
-        <v>1609340000000</v>
+        <v>621372736649.80676</v>
       </c>
     </row>
   </sheetData>
@@ -599,27 +602,26 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" customWidth="1"/>
+    <col min="2" max="2" width="26.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
-        <f>1.60934*10^12</f>
-        <v>1609340000000</v>
+        <v>621372736649.80676</v>
       </c>
     </row>
   </sheetData>

</xml_diff>